<commit_message>
change monthly examples to fom dates
</commit_message>
<xml_diff>
--- a/data_example/Gusher #1.xlsx
+++ b/data_example/Gusher #1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\apollo\data_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\PetroAlchemy\data_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ABCD37-8837-43A7-9106-6DADBA9A787F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B4112F-E268-44F8-9CD6-893741E7E5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,18 +387,18 @@
   <dimension ref="A1:D602"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="M114" sqref="M114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,12 +412,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>43942</v>
+        <v>43922</v>
       </c>
       <c r="C2" s="2">
         <v>60000</v>
@@ -426,12 +426,12 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>43972</v>
+        <v>43952</v>
       </c>
       <c r="C3" s="2">
         <v>43160.815662620771</v>
@@ -440,12 +440,12 @@
         <v>114327.95584781964</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>44003</v>
+        <v>43983</v>
       </c>
       <c r="C4" s="2">
         <v>33874.382624922247</v>
@@ -454,12 +454,12 @@
         <v>108904.55047242431</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>44033</v>
+        <v>44013</v>
       </c>
       <c r="C5" s="2">
         <v>28083.618772691443</v>
@@ -468,12 +468,12 @@
         <v>103881.37065240332</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>44064</v>
+        <v>44044</v>
       </c>
       <c r="C6" s="2">
         <v>24209.859039003833</v>
@@ -482,12 +482,12 @@
         <v>99364.039562124555</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>44095</v>
+        <v>44075</v>
       </c>
       <c r="C7" s="2">
         <v>21262.154761991584</v>
@@ -496,12 +496,12 @@
         <v>95017.579697761103</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>44125</v>
+        <v>44105</v>
       </c>
       <c r="C8" s="2">
         <v>19068.178768682141</v>
@@ -510,12 +510,12 @@
         <v>91093.837468023019</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>44156</v>
+        <v>44136</v>
       </c>
       <c r="C9" s="2">
         <v>17265.131704811683</v>
@@ -524,12 +524,12 @@
         <v>87304.803026174181</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>44186</v>
+        <v>44166</v>
       </c>
       <c r="C10" s="2">
         <v>15798.99279703713</v>
@@ -538,12 +538,12 @@
         <v>83761.787323700963</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>44217</v>
+        <v>44197</v>
       </c>
       <c r="C11" s="2">
         <v>14690.234894058749</v>
@@ -552,12 +552,12 @@
         <v>80755.219638554787</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1">
-        <v>44248</v>
+        <v>44228</v>
       </c>
       <c r="C12" s="2">
         <v>13645.435289265435</v>
@@ -566,12 +566,12 @@
         <v>77623.135004052136</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1">
-        <v>44276</v>
+        <v>44256</v>
       </c>
       <c r="C13" s="2">
         <v>12778.107732702645</v>
@@ -580,12 +580,12 @@
         <v>74773.095117536097</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1">
-        <v>44307</v>
+        <v>44287</v>
       </c>
       <c r="C14" s="2">
         <v>11999.999999999996</v>
@@ -594,12 +594,12 @@
         <v>72000.000000000015</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>44337</v>
+        <v>44317</v>
       </c>
       <c r="C15" s="2">
         <v>11339.682227244346</v>
@@ -608,12 +608,12 @@
         <v>69469.752959316567</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1">
-        <v>44368</v>
+        <v>44348</v>
       </c>
       <c r="C16" s="2">
         <v>10735.981550253629</v>
@@ -622,12 +622,12 @@
         <v>67001.413558663844</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1">
-        <v>44398</v>
+        <v>44378</v>
       </c>
       <c r="C17" s="2">
         <v>10198.745712160002</v>
@@ -636,12 +636,12 @@
         <v>64670.46639538095</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1">
-        <v>44429</v>
+        <v>44409</v>
       </c>
       <c r="C18" s="2">
         <v>9732.0570704709262</v>
@@ -650,12 +650,12 @@
         <v>62535.817704475943</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1">
-        <v>44460</v>
+        <v>44440</v>
       </c>
       <c r="C19" s="2">
         <v>9296.5254062478398</v>
@@ -664,12 +664,12 @@
         <v>60446.056018864016</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="1">
-        <v>44490</v>
+        <v>44470</v>
       </c>
       <c r="C20" s="2">
         <v>8913.8515920894315</v>
@@ -678,12 +678,12 @@
         <v>58528.079273322161</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="1">
-        <v>44521</v>
+        <v>44501</v>
       </c>
       <c r="C21" s="2">
         <v>8553.0646077705042</v>
@@ -692,12 +692,12 @@
         <v>56646.476068087133</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1">
-        <v>44551</v>
+        <v>44531</v>
       </c>
       <c r="C22" s="2">
         <v>8222.9166221572868</v>
@@ -706,12 +706,12 @@
         <v>54859.825214278761</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="1">
-        <v>44582</v>
+        <v>44562</v>
       </c>
       <c r="C23" s="2">
         <v>7947.8433398341813</v>
@@ -720,12 +720,12 @@
         <v>53322.299908643261</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>44613</v>
+        <v>44593</v>
       </c>
       <c r="C24" s="2">
         <v>7665.9124458538618</v>
@@ -734,12 +734,12 @@
         <v>51698.959670071767</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="1">
-        <v>44641</v>
+        <v>44621</v>
       </c>
       <c r="C25" s="2">
         <v>7413.1948972843165</v>
@@ -748,12 +748,12 @@
         <v>50201.974209917375</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="1">
-        <v>44672</v>
+        <v>44652</v>
       </c>
       <c r="C26" s="2">
         <v>7170.55415783238</v>
@@ -762,12 +762,12 @@
         <v>48726.654453032403</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1">
-        <v>44702</v>
+        <v>44682</v>
       </c>
       <c r="C27" s="2">
         <v>6951.7663202835483</v>
@@ -776,12 +776,12 @@
         <v>47363.874076335684</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="1">
-        <v>44733</v>
+        <v>44713</v>
       </c>
       <c r="C28" s="2">
         <v>6740.5532514355327</v>
@@ -790,12 +790,12 @@
         <v>46018.63244801604</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="1">
-        <v>44763</v>
+        <v>44743</v>
       </c>
       <c r="C29" s="2">
         <v>6542.9616641467073</v>
@@ -804,12 +804,12 @@
         <v>44733.498223928415</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="1">
-        <v>44794</v>
+        <v>44774</v>
       </c>
       <c r="C30" s="2">
         <v>6363.4768476079716</v>
@@ -818,12 +818,12 @@
         <v>43543.627189907544</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="1">
-        <v>44825</v>
+        <v>44805</v>
       </c>
       <c r="C31" s="2">
         <v>6189.0151676544556</v>
@@ -832,12 +832,12 @@
         <v>42366.423097778657</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1">
-        <v>44855</v>
+        <v>44835</v>
       </c>
       <c r="C32" s="2">
         <v>6029.8907472959609</v>
@@ -846,12 +846,12 @@
         <v>41274.932671352763</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1">
-        <v>44886</v>
+        <v>44866</v>
       </c>
       <c r="C33" s="2">
         <v>5874.6263681588889</v>
@@ -860,12 +860,12 @@
         <v>40193.577079744122</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1">
-        <v>44916</v>
+        <v>44896</v>
       </c>
       <c r="C34" s="2">
         <v>5727.8938981481297</v>
@@ -874,12 +874,12 @@
         <v>39156.847819388124</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="1">
-        <v>44947</v>
+        <v>44927</v>
       </c>
       <c r="C35" s="2">
         <v>5602.1079636469331</v>
@@ -888,12 +888,12 @@
         <v>38256.726665403032</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="1">
-        <v>44978</v>
+        <v>44958</v>
       </c>
       <c r="C36" s="2">
         <v>5469.7337301142952</v>
@@ -902,12 +902,12 @@
         <v>37298.187575428863</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="1">
-        <v>45006</v>
+        <v>44986</v>
       </c>
       <c r="C37" s="2">
         <v>5348.006418813231</v>
@@ -916,12 +916,12 @@
         <v>36406.63512513294</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="1">
-        <v>45037</v>
+        <v>45017</v>
       </c>
       <c r="C38" s="2">
         <v>5228.3148592548632</v>
@@ -930,12 +930,12 @@
         <v>35520.658605535471</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>4</v>
       </c>
       <c r="B39" s="1">
-        <v>45067</v>
+        <v>45047</v>
       </c>
       <c r="C39" s="2">
         <v>5117.9531627567831</v>
@@ -944,12 +944,12 @@
         <v>34695.653261522821</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="1">
-        <v>45098</v>
+        <v>45078</v>
       </c>
       <c r="C40" s="2">
         <v>5009.1598434259577</v>
@@ -958,12 +958,12 @@
         <v>33874.895485305024</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1">
-        <v>45128</v>
+        <v>45108</v>
       </c>
       <c r="C41" s="2">
         <v>4905.3278212452688</v>
@@ -972,12 +972,12 @@
         <v>33084.767875412785</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="1">
-        <v>45159</v>
+        <v>45139</v>
       </c>
       <c r="C42" s="2">
         <v>4809.2474424837019</v>
@@ -986,12 +986,12 @@
         <v>32347.831504967631</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="1">
-        <v>45190</v>
+        <v>45170</v>
       </c>
       <c r="C43" s="2">
         <v>4714.2110006585699</v>
@@ -1000,12 +1000,12 @@
         <v>31613.543011386279</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>4</v>
       </c>
       <c r="B44" s="1">
-        <v>45220</v>
+        <v>45200</v>
       </c>
       <c r="C44" s="2">
         <v>4626.0857675652378</v>
@@ -1014,12 +1014,12 @@
         <v>30928.005633539047</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="1">
-        <v>45251</v>
+        <v>45231</v>
       </c>
       <c r="C45" s="2">
         <v>4538.7443896170898</v>
@@ -1028,12 +1028,12 @@
         <v>30244.270721046094</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="1">
-        <v>45281</v>
+        <v>45261</v>
       </c>
       <c r="C46" s="2">
         <v>4454.9505114015838</v>
@@ -1042,12 +1042,12 @@
         <v>29584.403843647731</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>4</v>
       </c>
       <c r="B47" s="1">
-        <v>45312</v>
+        <v>45292</v>
       </c>
       <c r="C47" s="2">
         <v>4379.5810231959167</v>
@@ -1056,12 +1056,12 @@
         <v>28987.714215519707</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="1">
-        <v>45343</v>
+        <v>45323</v>
       </c>
       <c r="C48" s="2">
         <v>4302.0501135676614</v>
@@ -1070,12 +1070,12 @@
         <v>28370.890796377716</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="1">
-        <v>45372</v>
+        <v>45352</v>
       </c>
       <c r="C49" s="2">
         <v>4229.8371956410401</v>
@@ -1084,12 +1084,12 @@
         <v>27793.717689885903</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50" s="1">
-        <v>45403</v>
+        <v>45383</v>
       </c>
       <c r="C50" s="2">
         <v>4157.9617089268777</v>
@@ -1098,12 +1098,12 @@
         <v>27216.794585512773</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51" s="1">
-        <v>45433</v>
+        <v>45413</v>
       </c>
       <c r="C51" s="2">
         <v>4090.9135421190963</v>
@@ -1112,12 +1112,12 @@
         <v>26676.509544861157</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>4</v>
       </c>
       <c r="B52" s="1">
-        <v>45464</v>
+        <v>45444</v>
       </c>
       <c r="C52" s="2">
         <v>4024.0803710605992</v>
@@ -1126,12 +1126,12 @@
         <v>26136.022126006854</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="1">
-        <v>45494</v>
+        <v>45474</v>
       </c>
       <c r="C53" s="2">
         <v>3959.6031010978195</v>
@@ -1140,12 +1140,12 @@
         <v>25612.845263145267</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>4</v>
       </c>
       <c r="B54" s="1">
-        <v>45525</v>
+        <v>45505</v>
       </c>
       <c r="C54" s="2">
         <v>3899.3301981175891</v>
@@ -1154,12 +1154,12 @@
         <v>25122.317209149445</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="1">
-        <v>45556</v>
+        <v>45536</v>
       </c>
       <c r="C55" s="2">
         <v>3839.1294750107263</v>
@@ -1168,12 +1168,12 @@
         <v>24631.042452303358</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>4</v>
       </c>
       <c r="B56" s="1">
-        <v>45586</v>
+        <v>45566</v>
       </c>
       <c r="C56" s="2">
         <v>3782.7832220387268</v>
@@ -1182,12 +1182,12 @@
         <v>24170.087538137112</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="1">
-        <v>45617</v>
+        <v>45597</v>
       </c>
       <c r="C57" s="2">
         <v>3726.436010733551</v>
@@ -1196,12 +1196,12 @@
         <v>23708.100027409469</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>4</v>
       </c>
       <c r="B58" s="1">
-        <v>45647</v>
+        <v>45627</v>
       </c>
       <c r="C58" s="2">
         <v>3671.9029091902471</v>
@@ -1210,12 +1210,12 @@
         <v>23260.080921219069</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>4</v>
       </c>
       <c r="B59" s="1">
-        <v>45678</v>
+        <v>45658</v>
       </c>
       <c r="C59" s="2">
         <v>3624.1325673221227</v>
@@ -1224,12 +1224,12 @@
         <v>22866.946417852152</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>4</v>
       </c>
       <c r="B60" s="1">
-        <v>45709</v>
+        <v>45689</v>
       </c>
       <c r="C60" s="2">
         <v>3572.8118625373395</v>
@@ -1238,12 +1238,12 @@
         <v>22443.950706748976</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>4</v>
       </c>
       <c r="B61" s="1">
-        <v>45737</v>
+        <v>45717</v>
       </c>
       <c r="C61" s="2">
         <v>3524.6443002698593</v>
@@ -1252,12 +1252,12 @@
         <v>22046.39434781433</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>4</v>
       </c>
       <c r="B62" s="1">
-        <v>45768</v>
+        <v>45748</v>
       </c>
       <c r="C62" s="2">
         <v>3476.3473864078578</v>
@@ -1266,12 +1266,12 @@
         <v>21647.293410733619</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>4</v>
       </c>
       <c r="B63" s="1">
-        <v>45798</v>
+        <v>45778</v>
       </c>
       <c r="C63" s="2">
         <v>3430.972946136937</v>
@@ -1280,12 +1280,12 @@
         <v>21271.959395073718</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>4</v>
       </c>
       <c r="B64" s="1">
-        <v>45829</v>
+        <v>45809</v>
       </c>
       <c r="C64" s="2">
         <v>3385.4330702277389</v>
@@ -1294,12 +1294,12 @@
         <v>20894.935847269873</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>4</v>
       </c>
       <c r="B65" s="1">
-        <v>45859</v>
+        <v>45839</v>
       </c>
       <c r="C65" s="2">
         <v>3341.2021583438586</v>
@@ -1308,12 +1308,12 @@
         <v>20528.491496339779</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>4</v>
       </c>
       <c r="B66" s="1">
-        <v>45890</v>
+        <v>45870</v>
       </c>
       <c r="C66" s="2">
         <v>3299.5904102215286</v>
@@ -1322,12 +1322,12 @@
         <v>20183.560139545436</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>4</v>
       </c>
       <c r="B67" s="1">
-        <v>45921</v>
+        <v>45901</v>
       </c>
       <c r="C67" s="2">
         <v>3257.7711869327336</v>
@@ -1336,12 +1336,12 @@
         <v>19836.771838737623</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>4</v>
       </c>
       <c r="B68" s="1">
-        <v>45951</v>
+        <v>45931</v>
       </c>
       <c r="C68" s="2">
         <v>3218.395069203681</v>
@@ -1350,12 +1350,12 @@
         <v>19510.158340664449</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>4</v>
       </c>
       <c r="B69" s="1">
-        <v>45982</v>
+        <v>45962</v>
       </c>
       <c r="C69" s="2">
         <v>3178.7901888826686</v>
@@ -1364,12 +1364,12 @@
         <v>19181.605010899191</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>4</v>
       </c>
       <c r="B70" s="1">
-        <v>46012</v>
+        <v>45992</v>
       </c>
       <c r="C70" s="2">
         <v>3140.2419209617742</v>
@@ -1378,12 +1378,12 @@
         <v>18861.815681757118</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>4</v>
       </c>
       <c r="B71" s="1">
-        <v>46043</v>
+        <v>46023</v>
       </c>
       <c r="C71" s="2">
         <v>3106.2965463437013</v>
@@ -1392,12 +1392,12 @@
         <v>18580.241532104785</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>4</v>
       </c>
       <c r="B72" s="1">
-        <v>46074</v>
+        <v>46054</v>
       </c>
       <c r="C72" s="2">
         <v>3069.6425563259677</v>
@@ -1406,12 +1406,12 @@
         <v>18276.264945493571</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>4</v>
       </c>
       <c r="B73" s="1">
-        <v>46102</v>
+        <v>46082</v>
       </c>
       <c r="C73" s="2">
         <v>3035.064668823276</v>
@@ -1420,12 +1420,12 @@
         <v>17989.599367478037</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>4</v>
       </c>
       <c r="B74" s="1">
-        <v>46133</v>
+        <v>46113</v>
       </c>
       <c r="C74" s="2">
         <v>3000.2220327931291</v>
@@ -1434,12 +1434,12 @@
         <v>17700.862847900458</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>4</v>
       </c>
       <c r="B75" s="1">
-        <v>46163</v>
+        <v>46143</v>
       </c>
       <c r="C75" s="2">
         <v>2967.3301771405063</v>
@@ -1448,12 +1448,12 @@
         <v>17428.435587276392</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>4</v>
       </c>
       <c r="B76" s="1">
-        <v>46194</v>
+        <v>46174</v>
       </c>
       <c r="C76" s="2">
         <v>2934.1641925311383</v>
@@ -1462,12 +1462,12 @@
         <v>17153.907966165207</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>4</v>
       </c>
       <c r="B77" s="1">
-        <v>46224</v>
+        <v>46204</v>
       </c>
       <c r="C77" s="2">
         <v>2901.8029513083861</v>
@@ -1476,12 +1476,12 @@
         <v>16886.234379813792</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>4</v>
       </c>
       <c r="B78" s="1">
-        <v>46255</v>
+        <v>46235</v>
       </c>
       <c r="C78" s="2">
         <v>2871.223780154085</v>
@@ -1490,12 +1490,12 @@
         <v>16633.501737781644</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>4</v>
       </c>
       <c r="B79" s="1">
-        <v>46286</v>
+        <v>46266</v>
       </c>
       <c r="C79" s="2">
         <v>2840.3604907030794</v>
@@ -1504,12 +1504,12 @@
         <v>16378.643893044667</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>4</v>
       </c>
       <c r="B80" s="1">
-        <v>46316</v>
+        <v>46296</v>
       </c>
       <c r="C80" s="2">
         <v>2811.1791339677443</v>
@@ -1518,12 +1518,12 @@
         <v>16137.903981516491</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>4</v>
       </c>
       <c r="B81" s="1">
-        <v>46347</v>
+        <v>46327</v>
       </c>
       <c r="C81" s="2">
         <v>2781.7092797344399</v>
@@ -1532,12 +1532,12 @@
         <v>15895.033095990188</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>4</v>
       </c>
       <c r="B82" s="1">
-        <v>46377</v>
+        <v>46357</v>
       </c>
       <c r="C82" s="2">
         <v>2752.9106407969034</v>
@@ -1546,12 +1546,12 @@
         <v>15657.958069716771</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>4</v>
       </c>
       <c r="B83" s="1">
-        <v>46408</v>
+        <v>46388</v>
       </c>
       <c r="C83" s="2">
         <v>2727.4564572752206</v>
@@ -1560,12 +1560,12 @@
         <v>15448.650508973527</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>4</v>
       </c>
       <c r="B84" s="1">
-        <v>46439</v>
+        <v>46419</v>
       </c>
       <c r="C84" s="2">
         <v>2699.8717223385274</v>
@@ -1574,12 +1574,12 @@
         <v>15222.0919975096</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>4</v>
       </c>
       <c r="B85" s="1">
-        <v>46467</v>
+        <v>46447</v>
       </c>
       <c r="C85" s="2">
         <v>2673.7544087928486</v>
@@ -1588,12 +1588,12 @@
         <v>15007.860984104631</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>4</v>
       </c>
       <c r="B86" s="1">
-        <v>46498</v>
+        <v>46478</v>
       </c>
       <c r="C86" s="2">
         <v>2647.3435332948147</v>
@@ -1602,12 +1602,12 @@
         <v>14791.51268019244</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>4</v>
       </c>
       <c r="B87" s="1">
-        <v>46528</v>
+        <v>46508</v>
       </c>
       <c r="C87" s="2">
         <v>2622.3248813265582</v>
@@ -1616,12 +1616,12 @@
         <v>14586.855415177288</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>4</v>
       </c>
       <c r="B88" s="1">
-        <v>46559</v>
+        <v>46539</v>
       </c>
       <c r="C88" s="2">
         <v>2597.0124180128419</v>
@@ -1630,12 +1630,12 @@
         <v>14380.095163007114</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>4</v>
       </c>
       <c r="B89" s="1">
-        <v>46589</v>
+        <v>46569</v>
       </c>
       <c r="C89" s="2">
         <v>2572.2313334494697</v>
@@ -1644,12 +1644,12 @@
         <v>14177.984480816636</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>4</v>
       </c>
       <c r="B90" s="1">
-        <v>46620</v>
+        <v>46600</v>
       </c>
       <c r="C90" s="2">
         <v>2548.7395222318582</v>
@@ -1658,12 +1658,12 @@
         <v>13986.686184480588</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>4</v>
       </c>
       <c r="B91" s="1">
-        <v>46651</v>
+        <v>46631</v>
       </c>
       <c r="C91" s="2">
         <v>2524.95497508581</v>
@@ -1672,12 +1672,12 @@
         <v>13793.313583223668</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>4</v>
       </c>
       <c r="B92" s="1">
-        <v>46681</v>
+        <v>46661</v>
       </c>
       <c r="C92" s="2">
         <v>2502.3976055023481</v>
@@ -1686,12 +1686,12 @@
         <v>13610.21939470976</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>4</v>
       </c>
       <c r="B93" s="1">
-        <v>46712</v>
+        <v>46692</v>
       </c>
       <c r="C93" s="2">
         <v>2479.5489932910177</v>
@@ -1700,12 +1700,12 @@
         <v>13425.073724900643</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>4</v>
       </c>
       <c r="B94" s="1">
-        <v>46742</v>
+        <v>46722</v>
       </c>
       <c r="C94" s="2">
         <v>2457.1543792664284</v>
@@ -1714,12 +1714,12 @@
         <v>13243.925201397713</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>4</v>
       </c>
       <c r="B95" s="1">
-        <v>46773</v>
+        <v>46753</v>
       </c>
       <c r="C95" s="2">
         <v>2436.6033612929309</v>
@@ -1728,12 +1728,12 @@
         <v>13077.977995323365</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>4</v>
       </c>
       <c r="B96" s="1">
-        <v>46804</v>
+        <v>46784</v>
       </c>
       <c r="C96" s="2">
         <v>2415.048770793398</v>
@@ -1742,12 +1742,12 @@
         <v>12904.235395049453</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>4</v>
       </c>
       <c r="B97" s="1">
-        <v>46833</v>
+        <v>46813</v>
       </c>
       <c r="C97" s="2">
         <v>2394.5848278804674</v>
@@ -1756,12 +1756,12 @@
         <v>12739.586995577634</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>4</v>
       </c>
       <c r="B98" s="1">
-        <v>46864</v>
+        <v>46844</v>
       </c>
       <c r="C98" s="2">
         <v>2373.8353636647676</v>
@@ -1770,12 +1770,12 @@
         <v>12572.95358673708</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>4</v>
       </c>
       <c r="B99" s="1">
-        <v>46894</v>
+        <v>46874</v>
       </c>
       <c r="C99" s="2">
         <v>2354.1280990180703</v>
@@ -1784,12 +1784,12 @@
         <v>12414.990965942066</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>4</v>
       </c>
       <c r="B100" s="1">
-        <v>46925</v>
+        <v>46905</v>
       </c>
       <c r="C100" s="2">
         <v>2334.1382123152416</v>
@@ -1798,12 +1798,12 @@
         <v>12255.072825063806</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>4</v>
       </c>
       <c r="B101" s="1">
-        <v>46955</v>
+        <v>46935</v>
       </c>
       <c r="C101" s="2">
         <v>2314.5179928240882</v>
@@ -1812,12 +1812,12 @@
         <v>12098.42525850685</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>4</v>
       </c>
       <c r="B102" s="1">
-        <v>46986</v>
+        <v>46966</v>
       </c>
       <c r="C102" s="2">
         <v>2295.8728012978095</v>
@@ -1826,12 +1826,12 @@
         <v>11949.85886911066</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>4</v>
       </c>
       <c r="B103" s="1">
-        <v>47017</v>
+        <v>46997</v>
       </c>
       <c r="C103" s="2">
         <v>2276.9498246841094</v>
@@ -1840,12 +1840,12 @@
         <v>11799.383479764656</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>4</v>
       </c>
       <c r="B104" s="1">
-        <v>47047</v>
+        <v>47027</v>
       </c>
       <c r="C104" s="2">
         <v>2258.9608657415297</v>
@@ -1854,12 +1854,12 @@
         <v>11656.627923996093</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>4</v>
       </c>
       <c r="B105" s="1">
-        <v>47078</v>
+        <v>47058</v>
       </c>
       <c r="C105" s="2">
         <v>2240.6975677051687</v>
@@ -1868,12 +1868,12 @@
         <v>11511.99519701296</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>4</v>
       </c>
       <c r="B106" s="1">
-        <v>47108</v>
+        <v>47088</v>
       </c>
       <c r="C106" s="2">
         <v>2222.755990971224</v>
@@ -1882,12 +1882,12 @@
         <v>11370.212554167718</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>4</v>
       </c>
       <c r="B107" s="1">
-        <v>47139</v>
+        <v>47119</v>
       </c>
       <c r="C107" s="2">
         <v>2206.8199997418346</v>
@@ -1896,12 +1896,12 @@
         <v>11244.536704426744</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>4</v>
       </c>
       <c r="B108" s="1">
-        <v>47170</v>
+        <v>47150</v>
       </c>
       <c r="C108" s="2">
         <v>2189.4670247166309</v>
@@ -1910,12 +1910,12 @@
         <v>11107.968799915576</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>4</v>
       </c>
       <c r="B109" s="1">
-        <v>47198</v>
+        <v>47178</v>
       </c>
       <c r="C109" s="2">
         <v>2172.9570579669607</v>
@@ -1924,12 +1924,12 @@
         <v>10978.315555666341</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>4</v>
       </c>
       <c r="B110" s="1">
-        <v>47229</v>
+        <v>47209</v>
       </c>
       <c r="C110" s="2">
         <v>2156.1818355339674</v>
@@ -1938,12 +1938,12 @@
         <v>10846.865853672081</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>4</v>
       </c>
       <c r="B111" s="1">
-        <v>47259</v>
+        <v>47239</v>
       </c>
       <c r="C111" s="2">
         <v>2140.2166073094268</v>
@@ -1952,12 +1952,12 @@
         <v>10722.037760622814</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>4</v>
       </c>
       <c r="B112" s="1">
-        <v>47290</v>
+        <v>47270</v>
       </c>
       <c r="C112" s="2">
         <v>2123.9899401304542</v>
@@ -1966,12 +1966,12 @@
         <v>10595.446174463636</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>4</v>
       </c>
       <c r="B113" s="1">
-        <v>47320</v>
+        <v>47300</v>
       </c>
       <c r="C113" s="2">
         <v>2108.0314926628262</v>
@@ -1980,12 +1980,12 @@
         <v>10471.22916084795</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>4</v>
       </c>
       <c r="B114" s="1">
-        <v>47351</v>
+        <v>47331</v>
       </c>
       <c r="C114" s="2">
         <v>2092.8368168764164</v>
@@ -1994,12 +1994,12 @@
         <v>10353.222758911235</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1">
-        <v>47382</v>
+        <v>47362</v>
       </c>
       <c r="C115" s="2">
         <v>2077.3865459836134</v>
@@ -2008,12 +2008,12 @@
         <v>10233.502568757174</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>4</v>
       </c>
       <c r="B116" s="1">
-        <v>47412</v>
+        <v>47392</v>
       </c>
       <c r="C116" s="2">
         <v>2062.6715591065931</v>
@@ -2022,12 +2022,12 @@
         <v>10119.739354443282</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>4</v>
       </c>
       <c r="B117" s="1">
-        <v>47443</v>
+        <v>47423</v>
       </c>
       <c r="C117" s="2">
         <v>2047.7048831864827</v>
@@ -2036,12 +2036,12 @@
         <v>10004.295152680575</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>4</v>
       </c>
       <c r="B118" s="1">
-        <v>47473</v>
+        <v>47453</v>
       </c>
       <c r="C118" s="2">
         <v>2032.9750601387625</v>
@@ -2050,12 +2050,12 @@
         <v>9890.9437681630188</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>4</v>
       </c>
       <c r="B119" s="1">
-        <v>47504</v>
+        <v>47484</v>
       </c>
       <c r="C119" s="2">
         <v>2019.8695029548057</v>
@@ -2064,12 +2064,12 @@
         <v>9790.3175617540364</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>4</v>
       </c>
       <c r="B120" s="1">
-        <v>47535</v>
+        <v>47515</v>
       </c>
       <c r="C120" s="2">
         <v>2005.57475287183</v>
@@ -2078,2412 +2078,2412 @@
         <v>9680.8074813973872</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B121" s="1"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B122" s="1"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B123" s="1"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B124" s="1"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B125" s="1"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B126" s="1"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B127" s="1"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B128" s="1"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B129" s="1"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B130" s="1"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B131" s="1"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B132" s="1"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B133" s="1"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B134" s="1"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B135" s="1"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B136" s="1"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B137" s="1"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B138" s="1"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B139" s="1"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B140" s="1"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B141" s="1"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B142" s="1"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B143" s="1"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B144" s="1"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B145" s="1"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B146" s="1"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B147" s="1"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B148" s="1"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B149" s="1"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B150" s="1"/>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B151" s="1"/>
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B152" s="1"/>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B153" s="1"/>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B154" s="1"/>
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B155" s="1"/>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B156" s="1"/>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B157" s="1"/>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B158" s="1"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B159" s="1"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B160" s="1"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B161" s="1"/>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B162" s="1"/>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B163" s="1"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B164" s="1"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B165" s="1"/>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B166" s="1"/>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B167" s="1"/>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B168" s="1"/>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B169" s="1"/>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B170" s="1"/>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B171" s="1"/>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B172" s="1"/>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B173" s="1"/>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B174" s="1"/>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B175" s="1"/>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B176" s="1"/>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B177" s="1"/>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B178" s="1"/>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B179" s="1"/>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B180" s="1"/>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B181" s="1"/>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B182" s="1"/>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B183" s="1"/>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B184" s="1"/>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B185" s="1"/>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B186" s="1"/>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B187" s="1"/>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B188" s="1"/>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B189" s="1"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B190" s="1"/>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B191" s="1"/>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B192" s="1"/>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B193" s="1"/>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B194" s="1"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B195" s="1"/>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B196" s="1"/>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B197" s="1"/>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B198" s="1"/>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B199" s="1"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B200" s="1"/>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B201" s="1"/>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B202" s="1"/>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B203" s="1"/>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B204" s="1"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B205" s="1"/>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B206" s="1"/>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B207" s="1"/>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B208" s="1"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B209" s="1"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B210" s="1"/>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B211" s="1"/>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B212" s="1"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B213" s="1"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B214" s="1"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B215" s="1"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B216" s="1"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B217" s="1"/>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B218" s="1"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B219" s="1"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B220" s="1"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B221" s="1"/>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B222" s="1"/>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B223" s="1"/>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B224" s="1"/>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B225" s="1"/>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B226" s="1"/>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B227" s="1"/>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B228" s="1"/>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B229" s="1"/>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B230" s="1"/>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B231" s="1"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B232" s="1"/>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B233" s="1"/>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B234" s="1"/>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B235" s="1"/>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B236" s="1"/>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B237" s="1"/>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B238" s="1"/>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B239" s="1"/>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B240" s="1"/>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B241" s="1"/>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B242" s="1"/>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B243" s="1"/>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B244" s="1"/>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B245" s="1"/>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B246" s="1"/>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B247" s="1"/>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B248" s="1"/>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B249" s="1"/>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B250" s="1"/>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B251" s="1"/>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B252" s="1"/>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B253" s="1"/>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B254" s="1"/>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B255" s="1"/>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B256" s="1"/>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B257" s="1"/>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B258" s="1"/>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B259" s="1"/>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B260" s="1"/>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B261" s="1"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B262" s="1"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
     </row>
-    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B263" s="1"/>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B264" s="1"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B265" s="1"/>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B266" s="1"/>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
     </row>
-    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B267" s="1"/>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
     </row>
-    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B268" s="1"/>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
     </row>
-    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B269" s="1"/>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
     </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B270" s="1"/>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
     </row>
-    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B271" s="1"/>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B272" s="1"/>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B273" s="1"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B274" s="1"/>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
     </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B275" s="1"/>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B276" s="1"/>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B277" s="1"/>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B278" s="1"/>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
     </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B279" s="1"/>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B280" s="1"/>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B281" s="1"/>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B282" s="1"/>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
     </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B283" s="1"/>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B284" s="1"/>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B285" s="1"/>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B286" s="1"/>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B287" s="1"/>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B288" s="1"/>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B289" s="1"/>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B290" s="1"/>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B291" s="1"/>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B292" s="1"/>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B293" s="1"/>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B294" s="1"/>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B295" s="1"/>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B296" s="1"/>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B297" s="1"/>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B298" s="1"/>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B299" s="1"/>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B300" s="1"/>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
     </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B301" s="1"/>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B302" s="1"/>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B303" s="1"/>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B304" s="1"/>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
     </row>
-    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B305" s="1"/>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
     </row>
-    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B306" s="1"/>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B307" s="1"/>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
     </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B308" s="1"/>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
     </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B309" s="1"/>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
     </row>
-    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B310" s="1"/>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
     </row>
-    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B311" s="1"/>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
     </row>
-    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B312" s="1"/>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
     </row>
-    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B313" s="1"/>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B314" s="1"/>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
     </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B315" s="1"/>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
     </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B316" s="1"/>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
     </row>
-    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B317" s="1"/>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B318" s="1"/>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
     </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B319" s="1"/>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
     </row>
-    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B320" s="1"/>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B321" s="1"/>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
     </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B322" s="1"/>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
     </row>
-    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B323" s="1"/>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B324" s="1"/>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
     </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B325" s="1"/>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B326" s="1"/>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B327" s="1"/>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B328" s="1"/>
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B329" s="1"/>
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>
     </row>
-    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B330" s="1"/>
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
     </row>
-    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B331" s="1"/>
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
     </row>
-    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B332" s="1"/>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
     </row>
-    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B333" s="1"/>
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
     </row>
-    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B334" s="1"/>
       <c r="C334" s="2"/>
       <c r="D334" s="2"/>
     </row>
-    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B335" s="1"/>
       <c r="C335" s="2"/>
       <c r="D335" s="2"/>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B336" s="1"/>
       <c r="C336" s="2"/>
       <c r="D336" s="2"/>
     </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B337" s="1"/>
       <c r="C337" s="2"/>
       <c r="D337" s="2"/>
     </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B338" s="1"/>
       <c r="C338" s="2"/>
       <c r="D338" s="2"/>
     </row>
-    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B339" s="1"/>
       <c r="C339" s="2"/>
       <c r="D339" s="2"/>
     </row>
-    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B340" s="1"/>
       <c r="C340" s="2"/>
       <c r="D340" s="2"/>
     </row>
-    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B341" s="1"/>
       <c r="C341" s="2"/>
       <c r="D341" s="2"/>
     </row>
-    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B342" s="1"/>
       <c r="C342" s="2"/>
       <c r="D342" s="2"/>
     </row>
-    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B343" s="1"/>
       <c r="C343" s="2"/>
       <c r="D343" s="2"/>
     </row>
-    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B344" s="1"/>
       <c r="C344" s="2"/>
       <c r="D344" s="2"/>
     </row>
-    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B345" s="1"/>
       <c r="C345" s="2"/>
       <c r="D345" s="2"/>
     </row>
-    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B346" s="1"/>
       <c r="C346" s="2"/>
       <c r="D346" s="2"/>
     </row>
-    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B347" s="1"/>
       <c r="C347" s="2"/>
       <c r="D347" s="2"/>
     </row>
-    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B348" s="1"/>
       <c r="C348" s="2"/>
       <c r="D348" s="2"/>
     </row>
-    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B349" s="1"/>
       <c r="C349" s="2"/>
       <c r="D349" s="2"/>
     </row>
-    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B350" s="1"/>
       <c r="C350" s="2"/>
       <c r="D350" s="2"/>
     </row>
-    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B351" s="1"/>
       <c r="C351" s="2"/>
       <c r="D351" s="2"/>
     </row>
-    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B352" s="1"/>
       <c r="C352" s="2"/>
       <c r="D352" s="2"/>
     </row>
-    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B353" s="1"/>
       <c r="C353" s="2"/>
       <c r="D353" s="2"/>
     </row>
-    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B354" s="1"/>
       <c r="C354" s="2"/>
       <c r="D354" s="2"/>
     </row>
-    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B355" s="1"/>
       <c r="C355" s="2"/>
       <c r="D355" s="2"/>
     </row>
-    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B356" s="1"/>
       <c r="C356" s="2"/>
       <c r="D356" s="2"/>
     </row>
-    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B357" s="1"/>
       <c r="C357" s="2"/>
       <c r="D357" s="2"/>
     </row>
-    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B358" s="1"/>
       <c r="C358" s="2"/>
       <c r="D358" s="2"/>
     </row>
-    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B359" s="1"/>
       <c r="C359" s="2"/>
       <c r="D359" s="2"/>
     </row>
-    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B360" s="1"/>
       <c r="C360" s="2"/>
       <c r="D360" s="2"/>
     </row>
-    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B361" s="1"/>
       <c r="C361" s="2"/>
       <c r="D361" s="2"/>
     </row>
-    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B362" s="1"/>
       <c r="C362" s="2"/>
       <c r="D362" s="2"/>
     </row>
-    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B363" s="1"/>
       <c r="C363" s="2"/>
       <c r="D363" s="2"/>
     </row>
-    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B364" s="1"/>
       <c r="C364" s="2"/>
       <c r="D364" s="2"/>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B365" s="1"/>
       <c r="C365" s="2"/>
       <c r="D365" s="2"/>
     </row>
-    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B366" s="1"/>
       <c r="C366" s="2"/>
       <c r="D366" s="2"/>
     </row>
-    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B367" s="1"/>
       <c r="C367" s="2"/>
       <c r="D367" s="2"/>
     </row>
-    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B368" s="1"/>
       <c r="C368" s="2"/>
       <c r="D368" s="2"/>
     </row>
-    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B369" s="1"/>
       <c r="C369" s="2"/>
       <c r="D369" s="2"/>
     </row>
-    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B370" s="1"/>
       <c r="C370" s="2"/>
       <c r="D370" s="2"/>
     </row>
-    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B371" s="1"/>
       <c r="C371" s="2"/>
       <c r="D371" s="2"/>
     </row>
-    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B372" s="1"/>
       <c r="C372" s="2"/>
       <c r="D372" s="2"/>
     </row>
-    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B373" s="1"/>
       <c r="C373" s="2"/>
       <c r="D373" s="2"/>
     </row>
-    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B374" s="1"/>
       <c r="C374" s="2"/>
       <c r="D374" s="2"/>
     </row>
-    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B375" s="1"/>
       <c r="C375" s="2"/>
       <c r="D375" s="2"/>
     </row>
-    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B376" s="1"/>
       <c r="C376" s="2"/>
       <c r="D376" s="2"/>
     </row>
-    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B377" s="1"/>
       <c r="C377" s="2"/>
       <c r="D377" s="2"/>
     </row>
-    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B378" s="1"/>
       <c r="C378" s="2"/>
       <c r="D378" s="2"/>
     </row>
-    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B379" s="1"/>
       <c r="C379" s="2"/>
       <c r="D379" s="2"/>
     </row>
-    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B380" s="1"/>
       <c r="C380" s="2"/>
       <c r="D380" s="2"/>
     </row>
-    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B381" s="1"/>
       <c r="C381" s="2"/>
       <c r="D381" s="2"/>
     </row>
-    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B382" s="1"/>
       <c r="C382" s="2"/>
       <c r="D382" s="2"/>
     </row>
-    <row r="383" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B383" s="1"/>
       <c r="C383" s="2"/>
       <c r="D383" s="2"/>
     </row>
-    <row r="384" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B384" s="1"/>
       <c r="C384" s="2"/>
       <c r="D384" s="2"/>
     </row>
-    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B385" s="1"/>
       <c r="C385" s="2"/>
       <c r="D385" s="2"/>
     </row>
-    <row r="386" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B386" s="1"/>
       <c r="C386" s="2"/>
       <c r="D386" s="2"/>
     </row>
-    <row r="387" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B387" s="1"/>
       <c r="C387" s="2"/>
       <c r="D387" s="2"/>
     </row>
-    <row r="388" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="388" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B388" s="1"/>
       <c r="C388" s="2"/>
       <c r="D388" s="2"/>
     </row>
-    <row r="389" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="389" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B389" s="1"/>
       <c r="C389" s="2"/>
       <c r="D389" s="2"/>
     </row>
-    <row r="390" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="390" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B390" s="1"/>
       <c r="C390" s="2"/>
       <c r="D390" s="2"/>
     </row>
-    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="391" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B391" s="1"/>
       <c r="C391" s="2"/>
       <c r="D391" s="2"/>
     </row>
-    <row r="392" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="392" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B392" s="1"/>
       <c r="C392" s="2"/>
       <c r="D392" s="2"/>
     </row>
-    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="393" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B393" s="1"/>
       <c r="C393" s="2"/>
       <c r="D393" s="2"/>
     </row>
-    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="394" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B394" s="1"/>
       <c r="C394" s="2"/>
       <c r="D394" s="2"/>
     </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="395" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B395" s="1"/>
       <c r="C395" s="2"/>
       <c r="D395" s="2"/>
     </row>
-    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="396" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B396" s="1"/>
       <c r="C396" s="2"/>
       <c r="D396" s="2"/>
     </row>
-    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="397" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B397" s="1"/>
       <c r="C397" s="2"/>
       <c r="D397" s="2"/>
     </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="398" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B398" s="1"/>
       <c r="C398" s="2"/>
       <c r="D398" s="2"/>
     </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="399" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B399" s="1"/>
       <c r="C399" s="2"/>
       <c r="D399" s="2"/>
     </row>
-    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="400" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B400" s="1"/>
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>
     </row>
-    <row r="401" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B401" s="1"/>
       <c r="C401" s="2"/>
       <c r="D401" s="2"/>
     </row>
-    <row r="402" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B402" s="1"/>
       <c r="C402" s="2"/>
       <c r="D402" s="2"/>
     </row>
-    <row r="403" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B403" s="1"/>
       <c r="C403" s="2"/>
       <c r="D403" s="2"/>
     </row>
-    <row r="404" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B404" s="1"/>
       <c r="C404" s="2"/>
       <c r="D404" s="2"/>
     </row>
-    <row r="405" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B405" s="1"/>
       <c r="C405" s="2"/>
       <c r="D405" s="2"/>
     </row>
-    <row r="406" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B406" s="1"/>
       <c r="C406" s="2"/>
       <c r="D406" s="2"/>
     </row>
-    <row r="407" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B407" s="1"/>
       <c r="C407" s="2"/>
       <c r="D407" s="2"/>
     </row>
-    <row r="408" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B408" s="1"/>
       <c r="C408" s="2"/>
       <c r="D408" s="2"/>
     </row>
-    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B409" s="1"/>
       <c r="C409" s="2"/>
       <c r="D409" s="2"/>
     </row>
-    <row r="410" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B410" s="1"/>
       <c r="C410" s="2"/>
       <c r="D410" s="2"/>
     </row>
-    <row r="411" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B411" s="1"/>
       <c r="C411" s="2"/>
       <c r="D411" s="2"/>
     </row>
-    <row r="412" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B412" s="1"/>
       <c r="C412" s="2"/>
       <c r="D412" s="2"/>
     </row>
-    <row r="413" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B413" s="1"/>
       <c r="C413" s="2"/>
       <c r="D413" s="2"/>
     </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B414" s="1"/>
       <c r="C414" s="2"/>
       <c r="D414" s="2"/>
     </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B415" s="1"/>
       <c r="C415" s="2"/>
       <c r="D415" s="2"/>
     </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B416" s="1"/>
       <c r="C416" s="2"/>
       <c r="D416" s="2"/>
     </row>
-    <row r="417" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="417" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B417" s="1"/>
       <c r="C417" s="2"/>
       <c r="D417" s="2"/>
     </row>
-    <row r="418" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="418" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B418" s="1"/>
       <c r="C418" s="2"/>
       <c r="D418" s="2"/>
     </row>
-    <row r="419" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="419" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B419" s="1"/>
       <c r="C419" s="2"/>
       <c r="D419" s="2"/>
     </row>
-    <row r="420" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="420" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B420" s="1"/>
       <c r="C420" s="2"/>
       <c r="D420" s="2"/>
     </row>
-    <row r="421" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="421" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B421" s="1"/>
       <c r="C421" s="2"/>
       <c r="D421" s="2"/>
     </row>
-    <row r="422" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="422" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B422" s="1"/>
       <c r="C422" s="2"/>
       <c r="D422" s="2"/>
     </row>
-    <row r="423" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="423" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B423" s="1"/>
       <c r="C423" s="2"/>
       <c r="D423" s="2"/>
     </row>
-    <row r="424" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="424" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B424" s="1"/>
       <c r="C424" s="2"/>
       <c r="D424" s="2"/>
     </row>
-    <row r="425" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="425" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B425" s="1"/>
       <c r="C425" s="2"/>
       <c r="D425" s="2"/>
     </row>
-    <row r="426" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="426" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B426" s="1"/>
       <c r="C426" s="2"/>
       <c r="D426" s="2"/>
     </row>
-    <row r="427" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="427" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B427" s="1"/>
       <c r="C427" s="2"/>
       <c r="D427" s="2"/>
     </row>
-    <row r="428" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="428" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B428" s="1"/>
       <c r="C428" s="2"/>
       <c r="D428" s="2"/>
     </row>
-    <row r="429" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="429" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B429" s="1"/>
       <c r="C429" s="2"/>
       <c r="D429" s="2"/>
     </row>
-    <row r="430" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="430" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B430" s="1"/>
       <c r="C430" s="2"/>
       <c r="D430" s="2"/>
     </row>
-    <row r="431" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="431" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B431" s="1"/>
       <c r="C431" s="2"/>
       <c r="D431" s="2"/>
     </row>
-    <row r="432" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="432" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B432" s="1"/>
       <c r="C432" s="2"/>
       <c r="D432" s="2"/>
     </row>
-    <row r="433" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B433" s="1"/>
       <c r="C433" s="2"/>
       <c r="D433" s="2"/>
     </row>
-    <row r="434" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B434" s="1"/>
       <c r="C434" s="2"/>
       <c r="D434" s="2"/>
     </row>
-    <row r="435" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B435" s="1"/>
       <c r="C435" s="2"/>
       <c r="D435" s="2"/>
     </row>
-    <row r="436" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B436" s="1"/>
       <c r="C436" s="2"/>
       <c r="D436" s="2"/>
     </row>
-    <row r="437" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B437" s="1"/>
       <c r="C437" s="2"/>
       <c r="D437" s="2"/>
     </row>
-    <row r="438" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B438" s="1"/>
       <c r="C438" s="2"/>
       <c r="D438" s="2"/>
     </row>
-    <row r="439" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B439" s="1"/>
       <c r="C439" s="2"/>
       <c r="D439" s="2"/>
     </row>
-    <row r="440" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="440" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B440" s="1"/>
       <c r="C440" s="2"/>
       <c r="D440" s="2"/>
     </row>
-    <row r="441" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B441" s="1"/>
       <c r="C441" s="2"/>
       <c r="D441" s="2"/>
     </row>
-    <row r="442" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B442" s="1"/>
       <c r="C442" s="2"/>
       <c r="D442" s="2"/>
     </row>
-    <row r="443" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B443" s="1"/>
       <c r="C443" s="2"/>
       <c r="D443" s="2"/>
     </row>
-    <row r="444" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="444" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B444" s="1"/>
       <c r="C444" s="2"/>
       <c r="D444" s="2"/>
     </row>
-    <row r="445" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="445" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B445" s="1"/>
       <c r="C445" s="2"/>
       <c r="D445" s="2"/>
     </row>
-    <row r="446" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="446" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B446" s="1"/>
       <c r="C446" s="2"/>
       <c r="D446" s="2"/>
     </row>
-    <row r="447" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="447" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B447" s="1"/>
       <c r="C447" s="2"/>
       <c r="D447" s="2"/>
     </row>
-    <row r="448" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="448" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B448" s="1"/>
       <c r="C448" s="2"/>
       <c r="D448" s="2"/>
     </row>
-    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B449" s="1"/>
       <c r="C449" s="2"/>
       <c r="D449" s="2"/>
     </row>
-    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B450" s="1"/>
       <c r="C450" s="2"/>
       <c r="D450" s="2"/>
     </row>
-    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B451" s="1"/>
       <c r="C451" s="2"/>
       <c r="D451" s="2"/>
     </row>
-    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="452" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B452" s="1"/>
       <c r="C452" s="2"/>
       <c r="D452" s="2"/>
     </row>
-    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B453" s="1"/>
       <c r="C453" s="2"/>
       <c r="D453" s="2"/>
     </row>
-    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B454" s="1"/>
       <c r="C454" s="2"/>
       <c r="D454" s="2"/>
     </row>
-    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B455" s="1"/>
       <c r="C455" s="2"/>
       <c r="D455" s="2"/>
     </row>
-    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B456" s="1"/>
       <c r="C456" s="2"/>
       <c r="D456" s="2"/>
     </row>
-    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B457" s="1"/>
       <c r="C457" s="2"/>
       <c r="D457" s="2"/>
     </row>
-    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B458" s="1"/>
       <c r="C458" s="2"/>
       <c r="D458" s="2"/>
     </row>
-    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="459" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B459" s="1"/>
       <c r="C459" s="2"/>
       <c r="D459" s="2"/>
     </row>
-    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B460" s="1"/>
       <c r="C460" s="2"/>
       <c r="D460" s="2"/>
     </row>
-    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B461" s="1"/>
       <c r="C461" s="2"/>
       <c r="D461" s="2"/>
     </row>
-    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B462" s="1"/>
       <c r="C462" s="2"/>
       <c r="D462" s="2"/>
     </row>
-    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B463" s="1"/>
       <c r="C463" s="2"/>
       <c r="D463" s="2"/>
     </row>
-    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B464" s="1"/>
       <c r="C464" s="2"/>
       <c r="D464" s="2"/>
     </row>
-    <row r="465" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="465" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B465" s="1"/>
       <c r="C465" s="2"/>
       <c r="D465" s="2"/>
     </row>
-    <row r="466" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="466" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B466" s="1"/>
       <c r="C466" s="2"/>
       <c r="D466" s="2"/>
     </row>
-    <row r="467" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="467" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B467" s="1"/>
       <c r="C467" s="2"/>
       <c r="D467" s="2"/>
     </row>
-    <row r="468" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="468" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B468" s="1"/>
       <c r="C468" s="2"/>
       <c r="D468" s="2"/>
     </row>
-    <row r="469" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="469" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B469" s="1"/>
       <c r="C469" s="2"/>
       <c r="D469" s="2"/>
     </row>
-    <row r="470" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="470" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B470" s="1"/>
       <c r="C470" s="2"/>
       <c r="D470" s="2"/>
     </row>
-    <row r="471" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="471" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B471" s="1"/>
       <c r="C471" s="2"/>
       <c r="D471" s="2"/>
     </row>
-    <row r="472" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="472" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B472" s="1"/>
       <c r="C472" s="2"/>
       <c r="D472" s="2"/>
     </row>
-    <row r="473" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="473" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B473" s="1"/>
       <c r="C473" s="2"/>
       <c r="D473" s="2"/>
     </row>
-    <row r="474" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="474" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B474" s="1"/>
       <c r="C474" s="2"/>
       <c r="D474" s="2"/>
     </row>
-    <row r="475" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="475" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B475" s="1"/>
       <c r="C475" s="2"/>
       <c r="D475" s="2"/>
     </row>
-    <row r="476" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="476" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B476" s="1"/>
       <c r="C476" s="2"/>
       <c r="D476" s="2"/>
     </row>
-    <row r="477" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="477" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B477" s="1"/>
       <c r="C477" s="2"/>
       <c r="D477" s="2"/>
     </row>
-    <row r="478" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="478" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B478" s="1"/>
       <c r="C478" s="2"/>
       <c r="D478" s="2"/>
     </row>
-    <row r="479" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="479" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B479" s="1"/>
       <c r="C479" s="2"/>
       <c r="D479" s="2"/>
     </row>
-    <row r="480" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="480" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B480" s="1"/>
       <c r="C480" s="2"/>
       <c r="D480" s="2"/>
     </row>
-    <row r="481" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="481" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B481" s="1"/>
       <c r="C481" s="2"/>
       <c r="D481" s="2"/>
     </row>
-    <row r="482" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="482" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B482" s="1"/>
       <c r="C482" s="2"/>
       <c r="D482" s="2"/>
     </row>
-    <row r="483" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="483" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B483" s="1"/>
       <c r="C483" s="2"/>
       <c r="D483" s="2"/>
     </row>
-    <row r="484" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="484" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B484" s="1"/>
       <c r="C484" s="2"/>
       <c r="D484" s="2"/>
     </row>
-    <row r="485" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="485" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B485" s="1"/>
       <c r="C485" s="2"/>
       <c r="D485" s="2"/>
     </row>
-    <row r="486" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="486" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B486" s="1"/>
       <c r="C486" s="2"/>
       <c r="D486" s="2"/>
     </row>
-    <row r="487" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="487" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B487" s="1"/>
       <c r="C487" s="2"/>
       <c r="D487" s="2"/>
     </row>
-    <row r="488" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="488" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B488" s="1"/>
       <c r="C488" s="2"/>
       <c r="D488" s="2"/>
     </row>
-    <row r="489" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="489" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B489" s="1"/>
       <c r="C489" s="2"/>
       <c r="D489" s="2"/>
     </row>
-    <row r="490" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="490" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B490" s="1"/>
       <c r="C490" s="2"/>
       <c r="D490" s="2"/>
     </row>
-    <row r="491" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="491" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B491" s="1"/>
       <c r="C491" s="2"/>
       <c r="D491" s="2"/>
     </row>
-    <row r="492" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="492" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B492" s="1"/>
       <c r="C492" s="2"/>
       <c r="D492" s="2"/>
     </row>
-    <row r="493" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="493" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B493" s="1"/>
       <c r="C493" s="2"/>
       <c r="D493" s="2"/>
     </row>
-    <row r="494" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="494" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B494" s="1"/>
       <c r="C494" s="2"/>
       <c r="D494" s="2"/>
     </row>
-    <row r="495" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="495" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B495" s="1"/>
       <c r="C495" s="2"/>
       <c r="D495" s="2"/>
     </row>
-    <row r="496" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="496" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B496" s="1"/>
       <c r="C496" s="2"/>
       <c r="D496" s="2"/>
     </row>
-    <row r="497" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B497" s="1"/>
       <c r="C497" s="2"/>
       <c r="D497" s="2"/>
     </row>
-    <row r="498" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B498" s="1"/>
       <c r="C498" s="2"/>
       <c r="D498" s="2"/>
     </row>
-    <row r="499" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B499" s="1"/>
       <c r="C499" s="2"/>
       <c r="D499" s="2"/>
     </row>
-    <row r="500" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B500" s="1"/>
       <c r="C500" s="2"/>
       <c r="D500" s="2"/>
     </row>
-    <row r="501" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B501" s="1"/>
       <c r="C501" s="2"/>
       <c r="D501" s="2"/>
     </row>
-    <row r="502" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B502" s="1"/>
       <c r="C502" s="2"/>
       <c r="D502" s="2"/>
     </row>
-    <row r="503" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B503" s="1"/>
       <c r="C503" s="2"/>
       <c r="D503" s="2"/>
     </row>
-    <row r="504" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="504" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B504" s="1"/>
       <c r="C504" s="2"/>
       <c r="D504" s="2"/>
     </row>
-    <row r="505" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="505" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B505" s="1"/>
       <c r="C505" s="2"/>
       <c r="D505" s="2"/>
     </row>
-    <row r="506" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B506" s="1"/>
       <c r="C506" s="2"/>
       <c r="D506" s="2"/>
     </row>
-    <row r="507" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B507" s="1"/>
       <c r="C507" s="2"/>
       <c r="D507" s="2"/>
     </row>
-    <row r="508" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B508" s="1"/>
       <c r="C508" s="2"/>
       <c r="D508" s="2"/>
     </row>
-    <row r="509" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B509" s="1"/>
       <c r="C509" s="2"/>
       <c r="D509" s="2"/>
     </row>
-    <row r="510" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B510" s="1"/>
       <c r="C510" s="2"/>
       <c r="D510" s="2"/>
     </row>
-    <row r="511" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B511" s="1"/>
       <c r="C511" s="2"/>
       <c r="D511" s="2"/>
     </row>
-    <row r="512" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B512" s="1"/>
       <c r="C512" s="2"/>
       <c r="D512" s="2"/>
     </row>
-    <row r="513" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="513" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B513" s="1"/>
       <c r="C513" s="2"/>
       <c r="D513" s="2"/>
     </row>
-    <row r="514" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="514" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B514" s="1"/>
       <c r="C514" s="2"/>
       <c r="D514" s="2"/>
     </row>
-    <row r="515" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="515" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B515" s="1"/>
       <c r="C515" s="2"/>
       <c r="D515" s="2"/>
     </row>
-    <row r="516" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="516" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B516" s="1"/>
       <c r="C516" s="2"/>
       <c r="D516" s="2"/>
     </row>
-    <row r="517" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="517" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B517" s="1"/>
       <c r="C517" s="2"/>
       <c r="D517" s="2"/>
     </row>
-    <row r="518" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="518" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B518" s="1"/>
       <c r="C518" s="2"/>
       <c r="D518" s="2"/>
     </row>
-    <row r="519" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="519" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B519" s="1"/>
       <c r="C519" s="2"/>
       <c r="D519" s="2"/>
     </row>
-    <row r="520" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="520" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B520" s="1"/>
       <c r="C520" s="2"/>
       <c r="D520" s="2"/>
     </row>
-    <row r="521" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="521" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B521" s="1"/>
       <c r="C521" s="2"/>
       <c r="D521" s="2"/>
     </row>
-    <row r="522" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="522" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B522" s="1"/>
       <c r="C522" s="2"/>
       <c r="D522" s="2"/>
     </row>
-    <row r="523" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="523" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B523" s="1"/>
       <c r="C523" s="2"/>
       <c r="D523" s="2"/>
     </row>
-    <row r="524" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="524" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B524" s="1"/>
       <c r="C524" s="2"/>
       <c r="D524" s="2"/>
     </row>
-    <row r="525" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="525" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B525" s="1"/>
       <c r="C525" s="2"/>
       <c r="D525" s="2"/>
     </row>
-    <row r="526" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="526" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B526" s="1"/>
       <c r="C526" s="2"/>
       <c r="D526" s="2"/>
     </row>
-    <row r="527" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="527" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B527" s="1"/>
       <c r="C527" s="2"/>
       <c r="D527" s="2"/>
     </row>
-    <row r="528" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="528" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B528" s="1"/>
       <c r="C528" s="2"/>
       <c r="D528" s="2"/>
     </row>
-    <row r="529" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="529" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B529" s="1"/>
       <c r="C529" s="2"/>
       <c r="D529" s="2"/>
     </row>
-    <row r="530" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="530" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B530" s="1"/>
       <c r="C530" s="2"/>
       <c r="D530" s="2"/>
     </row>
-    <row r="531" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="531" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B531" s="1"/>
       <c r="C531" s="2"/>
       <c r="D531" s="2"/>
     </row>
-    <row r="532" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="532" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B532" s="1"/>
       <c r="C532" s="2"/>
       <c r="D532" s="2"/>
     </row>
-    <row r="533" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="533" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B533" s="1"/>
       <c r="C533" s="2"/>
       <c r="D533" s="2"/>
     </row>
-    <row r="534" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="534" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B534" s="1"/>
       <c r="C534" s="2"/>
       <c r="D534" s="2"/>
     </row>
-    <row r="535" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="535" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B535" s="1"/>
       <c r="C535" s="2"/>
       <c r="D535" s="2"/>
     </row>
-    <row r="536" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="536" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B536" s="1"/>
       <c r="C536" s="2"/>
       <c r="D536" s="2"/>
     </row>
-    <row r="537" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="537" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B537" s="1"/>
       <c r="C537" s="2"/>
       <c r="D537" s="2"/>
     </row>
-    <row r="538" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="538" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B538" s="1"/>
       <c r="C538" s="2"/>
       <c r="D538" s="2"/>
     </row>
-    <row r="539" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="539" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B539" s="1"/>
       <c r="C539" s="2"/>
       <c r="D539" s="2"/>
     </row>
-    <row r="540" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="540" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B540" s="1"/>
       <c r="C540" s="2"/>
       <c r="D540" s="2"/>
     </row>
-    <row r="541" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="541" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B541" s="1"/>
       <c r="C541" s="2"/>
       <c r="D541" s="2"/>
     </row>
-    <row r="542" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="542" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B542" s="1"/>
       <c r="C542" s="2"/>
       <c r="D542" s="2"/>
     </row>
-    <row r="543" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="543" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B543" s="1"/>
       <c r="C543" s="2"/>
       <c r="D543" s="2"/>
     </row>
-    <row r="544" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="544" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B544" s="1"/>
       <c r="C544" s="2"/>
       <c r="D544" s="2"/>
     </row>
-    <row r="545" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="545" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B545" s="1"/>
       <c r="C545" s="2"/>
       <c r="D545" s="2"/>
     </row>
-    <row r="546" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="546" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B546" s="1"/>
       <c r="C546" s="2"/>
       <c r="D546" s="2"/>
     </row>
-    <row r="547" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="547" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B547" s="1"/>
       <c r="C547" s="2"/>
       <c r="D547" s="2"/>
     </row>
-    <row r="548" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="548" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B548" s="1"/>
       <c r="C548" s="2"/>
       <c r="D548" s="2"/>
     </row>
-    <row r="549" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="549" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B549" s="1"/>
       <c r="C549" s="2"/>
       <c r="D549" s="2"/>
     </row>
-    <row r="550" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="550" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B550" s="1"/>
       <c r="C550" s="2"/>
       <c r="D550" s="2"/>
     </row>
-    <row r="551" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="551" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B551" s="1"/>
       <c r="C551" s="2"/>
       <c r="D551" s="2"/>
     </row>
-    <row r="552" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="552" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B552" s="1"/>
       <c r="C552" s="2"/>
       <c r="D552" s="2"/>
     </row>
-    <row r="553" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="553" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B553" s="1"/>
       <c r="C553" s="2"/>
       <c r="D553" s="2"/>
     </row>
-    <row r="554" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="554" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B554" s="1"/>
       <c r="C554" s="2"/>
       <c r="D554" s="2"/>
     </row>
-    <row r="555" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="555" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B555" s="1"/>
       <c r="C555" s="2"/>
       <c r="D555" s="2"/>
     </row>
-    <row r="556" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="556" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B556" s="1"/>
       <c r="C556" s="2"/>
       <c r="D556" s="2"/>
     </row>
-    <row r="557" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="557" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B557" s="1"/>
       <c r="C557" s="2"/>
       <c r="D557" s="2"/>
     </row>
-    <row r="558" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="558" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B558" s="1"/>
       <c r="C558" s="2"/>
       <c r="D558" s="2"/>
     </row>
-    <row r="559" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="559" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B559" s="1"/>
       <c r="C559" s="2"/>
       <c r="D559" s="2"/>
     </row>
-    <row r="560" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="560" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B560" s="1"/>
       <c r="C560" s="2"/>
       <c r="D560" s="2"/>
     </row>
-    <row r="561" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="561" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B561" s="1"/>
       <c r="C561" s="2"/>
       <c r="D561" s="2"/>
     </row>
-    <row r="562" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="562" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B562" s="1"/>
       <c r="C562" s="2"/>
       <c r="D562" s="2"/>
     </row>
-    <row r="563" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="563" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B563" s="1"/>
       <c r="C563" s="2"/>
       <c r="D563" s="2"/>
     </row>
-    <row r="564" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="564" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B564" s="1"/>
       <c r="C564" s="2"/>
       <c r="D564" s="2"/>
     </row>
-    <row r="565" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="565" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B565" s="1"/>
       <c r="C565" s="2"/>
       <c r="D565" s="2"/>
     </row>
-    <row r="566" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="566" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B566" s="1"/>
       <c r="C566" s="2"/>
       <c r="D566" s="2"/>
     </row>
-    <row r="567" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="567" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B567" s="1"/>
       <c r="C567" s="2"/>
       <c r="D567" s="2"/>
     </row>
-    <row r="568" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="568" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B568" s="1"/>
       <c r="C568" s="2"/>
       <c r="D568" s="2"/>
     </row>
-    <row r="569" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="569" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B569" s="1"/>
       <c r="C569" s="2"/>
       <c r="D569" s="2"/>
     </row>
-    <row r="570" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="570" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B570" s="1"/>
       <c r="C570" s="2"/>
       <c r="D570" s="2"/>
     </row>
-    <row r="571" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="571" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B571" s="1"/>
       <c r="C571" s="2"/>
       <c r="D571" s="2"/>
     </row>
-    <row r="572" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="572" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B572" s="1"/>
       <c r="C572" s="2"/>
       <c r="D572" s="2"/>
     </row>
-    <row r="573" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="573" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B573" s="1"/>
       <c r="C573" s="2"/>
       <c r="D573" s="2"/>
     </row>
-    <row r="574" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="574" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B574" s="1"/>
       <c r="C574" s="2"/>
       <c r="D574" s="2"/>
     </row>
-    <row r="575" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="575" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B575" s="1"/>
       <c r="C575" s="2"/>
       <c r="D575" s="2"/>
     </row>
-    <row r="576" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="576" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B576" s="1"/>
       <c r="C576" s="2"/>
       <c r="D576" s="2"/>
     </row>
-    <row r="577" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="577" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B577" s="1"/>
       <c r="C577" s="2"/>
       <c r="D577" s="2"/>
     </row>
-    <row r="578" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="578" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B578" s="1"/>
       <c r="C578" s="2"/>
       <c r="D578" s="2"/>
     </row>
-    <row r="579" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="579" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B579" s="1"/>
       <c r="C579" s="2"/>
       <c r="D579" s="2"/>
     </row>
-    <row r="580" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="580" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B580" s="1"/>
       <c r="C580" s="2"/>
       <c r="D580" s="2"/>
     </row>
-    <row r="581" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="581" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B581" s="1"/>
       <c r="C581" s="2"/>
       <c r="D581" s="2"/>
     </row>
-    <row r="582" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="582" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B582" s="1"/>
       <c r="C582" s="2"/>
       <c r="D582" s="2"/>
     </row>
-    <row r="583" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="583" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B583" s="1"/>
       <c r="C583" s="2"/>
       <c r="D583" s="2"/>
     </row>
-    <row r="584" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="584" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B584" s="1"/>
       <c r="C584" s="2"/>
       <c r="D584" s="2"/>
     </row>
-    <row r="585" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="585" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B585" s="1"/>
       <c r="C585" s="2"/>
       <c r="D585" s="2"/>
     </row>
-    <row r="586" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="586" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B586" s="1"/>
       <c r="C586" s="2"/>
       <c r="D586" s="2"/>
     </row>
-    <row r="587" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="587" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B587" s="1"/>
       <c r="C587" s="2"/>
       <c r="D587" s="2"/>
     </row>
-    <row r="588" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="588" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B588" s="1"/>
       <c r="C588" s="2"/>
       <c r="D588" s="2"/>
     </row>
-    <row r="589" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="589" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B589" s="1"/>
       <c r="C589" s="2"/>
       <c r="D589" s="2"/>
     </row>
-    <row r="590" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="590" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B590" s="1"/>
       <c r="C590" s="2"/>
       <c r="D590" s="2"/>
     </row>
-    <row r="591" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="591" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B591" s="1"/>
       <c r="C591" s="2"/>
       <c r="D591" s="2"/>
     </row>
-    <row r="592" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="592" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B592" s="1"/>
       <c r="C592" s="2"/>
       <c r="D592" s="2"/>
     </row>
-    <row r="593" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="593" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B593" s="1"/>
       <c r="C593" s="2"/>
       <c r="D593" s="2"/>
     </row>
-    <row r="594" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="594" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B594" s="1"/>
       <c r="C594" s="2"/>
       <c r="D594" s="2"/>
     </row>
-    <row r="595" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="595" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B595" s="1"/>
       <c r="C595" s="2"/>
       <c r="D595" s="2"/>
     </row>
-    <row r="596" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="596" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B596" s="1"/>
       <c r="C596" s="2"/>
       <c r="D596" s="2"/>
     </row>
-    <row r="597" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="597" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B597" s="1"/>
       <c r="C597" s="2"/>
       <c r="D597" s="2"/>
     </row>
-    <row r="598" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="598" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B598" s="1"/>
       <c r="C598" s="2"/>
       <c r="D598" s="2"/>
     </row>
-    <row r="599" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="599" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B599" s="1"/>
       <c r="C599" s="2"/>
       <c r="D599" s="2"/>
     </row>
-    <row r="600" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="600" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B600" s="1"/>
       <c r="C600" s="2"/>
       <c r="D600" s="2"/>
     </row>
-    <row r="601" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="601" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B601" s="1"/>
       <c r="C601" s="2"/>
       <c r="D601" s="2"/>
     </row>
-    <row r="602" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="602" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B602" s="1"/>
       <c r="C602" s="2"/>
       <c r="D602" s="2"/>

</xml_diff>